<commit_message>
Criando a tela 'Diario de Classe'
</commit_message>
<xml_diff>
--- a/arquivos salvos/base_dados_frequencia.xlsx
+++ b/arquivos salvos/base_dados_frequencia.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F165"/>
+  <dimension ref="A1:F169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4070,8 +4070,124 @@
           <t>P</t>
         </is>
       </c>
-      <c r="E165" t="inlineStr"/>
-      <c r="F165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>maria</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>2024-03-01</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>maria</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>2024-01-10</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Não tem</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Também não tem</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>maria</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>2024-10-07</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Testeeeee</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Testeeee</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>maria</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>2024-10-07</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Hoje teve aula</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Hoje Teve de fato aula</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Atualização da tela de matricula e correção de bugs
</commit_message>
<xml_diff>
--- a/arquivos salvos/base_dados_frequencia.xlsx
+++ b/arquivos salvos/base_dados_frequencia.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F169"/>
+  <dimension ref="A1:F183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4189,6 +4189,376 @@
         </is>
       </c>
     </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>44554</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>2024-10-10</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>323443</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>2024-10-10</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>44554</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>2024-10-11</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Cirio</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirio </t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>323443</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>2024-10-11</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Cirio</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirio </t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>44554</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>2024-10-14</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>323443</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>2024-10-14</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>44554</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>2024-08-15</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>niver nanzao</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>niver nanzao</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>323443</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>2024-08-15</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>niver nanzao</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>niver nanzao</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>44554</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>2024-08-16</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>323443</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>2024-08-16</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>44554</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>2024-08-19</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>323443</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>2024-08-19</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>44554</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>2024-08-20</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>323443</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>2024-08-20</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr"/>
+      <c r="F183" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>